<commit_message>
mise a jour du 30/07
</commit_message>
<xml_diff>
--- a/Religions/Lorentis Religions.xlsx
+++ b/Religions/Lorentis Religions.xlsx
@@ -954,7 +954,7 @@
   <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68 F68"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -998,7 +998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>93857</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>8114</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>7</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>50370</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>9</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>2209</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>10</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>11</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>12</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>13</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>14</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>15</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>16</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>17</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>19</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>20</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>21</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>22</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>23</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>24</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>25</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>26</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>27</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>28</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>29</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>30</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>31</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>32</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>33</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>34</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>35</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>36</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>37</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>38</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>39</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>40</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>41</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>42</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>43</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>44</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>45</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>46</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>47</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>48</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>49</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>50</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>51</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>52</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>53</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>54</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>55</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>80578</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>56</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>57</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>58</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>59</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>60</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>61</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>62</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>63</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>64</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>65</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>66</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>67</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>68</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>69</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>70</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>71</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>72</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>73</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>74</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>75</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>76</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>77</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>78</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>79</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>80</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>81</v>
       </c>

</xml_diff>